<commit_message>
Added the suggestions Franco made after the second midterm class. Week 8
</commit_message>
<xml_diff>
--- a/ModelsData/TidalData/24 hour tidal boundary time series.xlsx
+++ b/ModelsData/TidalData/24 hour tidal boundary time series.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Franco\from desktop 042312\DU\Teaching\18-19\Urban Ecohydraulics\Project data\tidal data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msc94\Documents\GitHub\GrandAnseBeach_SWMM\ModelsData\TidalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,18 +24,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>hour of day</t>
   </si>
   <si>
     <t>tidal elevation, m</t>
   </si>
+  <si>
+    <t>tidal elevation, ft</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,215 +350,316 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E8:F32"/>
+  <dimension ref="E8:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="10" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f>F9*0.3048</f>
+        <v>0.24384000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="11" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" ref="G10:G32" si="0">F10*0.3048</f>
+        <v>0.25908000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="12" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0.24993599999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E12">
         <v>3</v>
       </c>
       <c r="F12">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="13" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0.24384000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>4</v>
       </c>
       <c r="F13">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="14" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0.23774400000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E14">
         <v>5</v>
       </c>
       <c r="F14">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="15" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>0.24384000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E15">
         <v>6</v>
       </c>
       <c r="F15">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="16" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0.24993599999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E16">
         <v>7</v>
       </c>
       <c r="F16">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0.25908000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17">
         <v>8</v>
       </c>
       <c r="F17">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0.26517600000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E18">
         <v>9</v>
       </c>
       <c r="F18">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0.26822400000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>10</v>
       </c>
       <c r="F19">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0.27432000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>11</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>0.30480000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E21">
         <v>12</v>
       </c>
       <c r="F21">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>0.32004000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E22">
         <v>13</v>
       </c>
       <c r="F22">
         <v>1.02</v>
       </c>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>0.31089600000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E23">
         <v>14</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>0.30480000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E24">
         <v>15</v>
       </c>
       <c r="F24">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>0.27432000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>16</v>
       </c>
       <c r="F25">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>0.25908000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>17</v>
       </c>
       <c r="F26">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>0.24384000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>18</v>
       </c>
       <c r="F27">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>0.22860000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>19</v>
       </c>
       <c r="F28">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>0.21335999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E29">
         <v>20</v>
       </c>
       <c r="F29">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>0.19812000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>21</v>
       </c>
       <c r="F30">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="31" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>0.20726400000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E31">
         <v>22</v>
       </c>
       <c r="F31">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="32" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>0.21335999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E32">
         <v>23</v>
       </c>
       <c r="F32">
         <v>0.75</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>0.22860000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on the SWMM model
</commit_message>
<xml_diff>
--- a/ModelsData/TidalData/24 hour tidal boundary time series.xlsx
+++ b/ModelsData/TidalData/24 hour tidal boundary time series.xlsx
@@ -39,6 +39,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E8:G32"/>
+  <dimension ref="E8:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="H9" sqref="H9:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -363,7 +367,7 @@
     <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>0</v>
       </c>
@@ -374,7 +378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>0</v>
       </c>
@@ -385,8 +389,12 @@
         <f>F9*0.3048</f>
         <v>0.24384000000000003</v>
       </c>
-    </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="1">
+        <f>G9+16/12</f>
+        <v>1.5771733333333333</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>1</v>
       </c>
@@ -397,8 +405,12 @@
         <f t="shared" ref="G10:G32" si="0">F10*0.3048</f>
         <v>0.25908000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="1">
+        <f t="shared" ref="H10:H32" si="1">G10+16/12</f>
+        <v>1.5924133333333332</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E11">
         <v>2</v>
       </c>
@@ -409,8 +421,12 @@
         <f t="shared" si="0"/>
         <v>0.24993599999999999</v>
       </c>
-    </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5832693333333332</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E12">
         <v>3</v>
       </c>
@@ -421,8 +437,12 @@
         <f t="shared" si="0"/>
         <v>0.24384000000000003</v>
       </c>
-    </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5771733333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>4</v>
       </c>
@@ -433,8 +453,12 @@
         <f t="shared" si="0"/>
         <v>0.23774400000000001</v>
       </c>
-    </row>
-    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5710773333333332</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E14">
         <v>5</v>
       </c>
@@ -445,8 +469,12 @@
         <f t="shared" si="0"/>
         <v>0.24384000000000003</v>
       </c>
-    </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5771733333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E15">
         <v>6</v>
       </c>
@@ -457,8 +485,12 @@
         <f t="shared" si="0"/>
         <v>0.24993599999999999</v>
       </c>
-    </row>
-    <row r="16" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5832693333333332</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E16">
         <v>7</v>
       </c>
@@ -469,8 +501,12 @@
         <f t="shared" si="0"/>
         <v>0.25908000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5924133333333332</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17">
         <v>8</v>
       </c>
@@ -481,8 +517,12 @@
         <f t="shared" si="0"/>
         <v>0.26517600000000002</v>
       </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5985093333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E18">
         <v>9</v>
       </c>
@@ -493,8 +533,12 @@
         <f t="shared" si="0"/>
         <v>0.26822400000000002</v>
       </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6015573333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>10</v>
       </c>
@@ -505,8 +549,12 @@
         <f t="shared" si="0"/>
         <v>0.27432000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6076533333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>11</v>
       </c>
@@ -517,8 +565,12 @@
         <f t="shared" si="0"/>
         <v>0.30480000000000002</v>
       </c>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6381333333333332</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E21">
         <v>12</v>
       </c>
@@ -529,8 +581,12 @@
         <f t="shared" si="0"/>
         <v>0.32004000000000005</v>
       </c>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6533733333333334</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E22">
         <v>13</v>
       </c>
@@ -541,8 +597,12 @@
         <f t="shared" si="0"/>
         <v>0.31089600000000001</v>
       </c>
-    </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6442293333333333</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E23">
         <v>14</v>
       </c>
@@ -553,8 +613,12 @@
         <f t="shared" si="0"/>
         <v>0.30480000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6381333333333332</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E24">
         <v>15</v>
       </c>
@@ -565,8 +629,12 @@
         <f t="shared" si="0"/>
         <v>0.27432000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6076533333333334</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>16</v>
       </c>
@@ -577,8 +645,12 @@
         <f t="shared" si="0"/>
         <v>0.25908000000000003</v>
       </c>
-    </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5924133333333332</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>17</v>
       </c>
@@ -589,8 +661,12 @@
         <f t="shared" si="0"/>
         <v>0.24384000000000003</v>
       </c>
-    </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5771733333333333</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>18</v>
       </c>
@@ -601,8 +677,12 @@
         <f t="shared" si="0"/>
         <v>0.22860000000000003</v>
       </c>
-    </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5619333333333332</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>19</v>
       </c>
@@ -613,8 +693,12 @@
         <f t="shared" si="0"/>
         <v>0.21335999999999999</v>
       </c>
-    </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5466933333333333</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E29">
         <v>20</v>
       </c>
@@ -625,8 +709,12 @@
         <f t="shared" si="0"/>
         <v>0.19812000000000002</v>
       </c>
-    </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5314533333333333</v>
+      </c>
+    </row>
+    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>21</v>
       </c>
@@ -637,8 +725,12 @@
         <f t="shared" si="0"/>
         <v>0.20726400000000003</v>
       </c>
-    </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5405973333333334</v>
+      </c>
+    </row>
+    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E31">
         <v>22</v>
       </c>
@@ -649,8 +741,12 @@
         <f t="shared" si="0"/>
         <v>0.21335999999999999</v>
       </c>
-    </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5466933333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E32">
         <v>23</v>
       </c>
@@ -660,6 +756,10 @@
       <c r="G32">
         <f t="shared" si="0"/>
         <v>0.22860000000000003</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5619333333333332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Model and Figures
</commit_message>
<xml_diff>
--- a/ModelsData/TidalData/24 hour tidal boundary time series.xlsx
+++ b/ModelsData/TidalData/24 hour tidal boundary time series.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msc94\Documents\GitHub\GrandAnseBeach_SWMM\ModelsData\TidalData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gotmi\Documents\GitHub\GrandAnseBeach_SWMM\ModelsData\TidalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D06D3CE-2282-4E3B-BD70-E44DDA057028}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="28680" yWindow="1935" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>hour of day</t>
   </si>
@@ -34,13 +41,16 @@
   <si>
     <t>tidal elevation, ft</t>
   </si>
+  <si>
+    <t>CAT tidal elevation, ft</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -73,7 +83,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,11 +363,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E8:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:H32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,6 +387,9 @@
       <c r="G8" t="s">
         <v>2</v>
       </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E9">

</xml_diff>

<commit_message>
Finalized Climate Change Model
</commit_message>
<xml_diff>
--- a/ModelsData/TidalData/24 hour tidal boundary time series.xlsx
+++ b/ModelsData/TidalData/24 hour tidal boundary time series.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gotmi\Documents\GitHub\GrandAnseBeach_SWMM\ModelsData\TidalData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msc94\Documents\GitHub\GrandAnseBeach_SWMM\ModelsData\TidalData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D06D3CE-2282-4E3B-BD70-E44DDA057028}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1935" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1935" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
@@ -363,11 +362,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E8:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H9" sqref="H9:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>